<commit_message>
Swamy/11sep2022 s2 sql cosmos web api app 12sep2022 (#16)
* Initial Version

* Cosmos Db Initial Version

* Few Updates

* Creating the Cosmos Db using ARM Template

* Update README.md

* Update sql-server.parameters.json

* Verified the SQL Deployment using VS 2022

* Verified Blazor WASM

* Initial Version

* Removed unwanted images

* Few Changes
</commit_message>
<xml_diff>
--- a/csharp-corner/MSLearnModules.xlsx
+++ b/csharp-corner/MSLearnModules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LordKrishna\GitHub\speaker-series-2022\csharp-corner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035AA627-1576-4C46-8D6A-A17DA9C85AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C92729E-3C73-49DA-89BA-B1801CD7A22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>https://docs.microsoft.com/en-gb/learn/modules/provision-virtual-machines-azure/</t>
   </si>
@@ -34,13 +34,67 @@
   </si>
   <si>
     <t>Session 1</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/paths/az-204-implement-iaas-solutions/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/modules/publish-container-image-to-azure-container-registry/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/modules/create-run-container-images-azure-container-instances/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/paths/create-azure-app-service-web-apps/</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/modules/introduction-to-azure-app-service/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/modules/configure-web-app-settings/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/modules/scale-apps-app-service/</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/training/modules/understand-app-service-deployment-slots/</t>
+  </si>
+  <si>
+    <t>Session 2</t>
+  </si>
+  <si>
+    <t>Discussed on Web API, and Web Apps using .NET 6</t>
+  </si>
+  <si>
+    <t>Session 3</t>
+  </si>
+  <si>
+    <t>This session includes deployment of Web Api, and Web Apps inside Windows VM ()</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Scheduled</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +108,54 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFB9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,14 +163,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -86,6 +238,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFB9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -360,35 +517,310 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D3:E4"/>
+  <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="100.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="3.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="108.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="83" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D3" s="1" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="7">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="13"/>
+      <c r="G3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="7"/>
+      <c r="C4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="D4" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="D5" s="9" t="s">
         <v>2</v>
       </c>
+      <c r="E5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="7"/>
+      <c r="C6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="7"/>
+      <c r="C7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="15"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="13"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="C10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="15"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="13"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="7"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="13"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" s="7"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="13"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="7"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="13"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="7"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="13"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="7"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="13"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" s="7"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="13"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="7"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="13"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="7"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="13"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" s="7"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="13"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" s="7"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="13"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="7"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="13"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" s="7"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="13"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" s="7"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="13"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="7"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="13"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Session 4 -> C# Corner
</commit_message>
<xml_diff>
--- a/csharp-corner/MSLearnModules.xlsx
+++ b/csharp-corner/MSLearnModules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LordKrishna\GitHub\speaker-series-2022\csharp-corner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C92729E-3C73-49DA-89BA-B1801CD7A22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECB8D9D-BBC9-4376-834D-D2903A9AC0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>https://docs.microsoft.com/en-gb/learn/modules/provision-virtual-machines-azure/</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Scheduled</t>
+  </si>
+  <si>
+    <t>Session 4</t>
+  </si>
+  <si>
+    <t>Session 5</t>
   </si>
 </sst>
 </file>
@@ -123,7 +129,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFB9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -196,9 +208,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -230,6 +239,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -520,7 +538,7 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.3"/>
@@ -537,44 +555,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12"/>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -585,240 +603,248 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="13" t="s">
-        <v>7</v>
+      <c r="D6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="15"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="14"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="12"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>20</v>
+      <c r="E10" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="16" t="s">
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="15"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="14"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="12"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="12"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="12"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="12"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="12"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="12"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="12"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="12"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="12"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="13"/>
+      <c r="E24" s="12"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="12"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="12"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="13"/>
+      <c r="E28" s="12"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="12"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>

</xml_diff>

<commit_message>
Swamy/12oct2022 gettingstartedwithyourfirst microservicein net6 samosa chai net (#37)
* Initial Version

* Few Changes

* Updates

* Initial Version

* Documentation Updates

* Update data.json

* Session 4 -> C# Corner
</commit_message>
<xml_diff>
--- a/csharp-corner/MSLearnModules.xlsx
+++ b/csharp-corner/MSLearnModules.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LordKrishna\GitHub\speaker-series-2022\csharp-corner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C92729E-3C73-49DA-89BA-B1801CD7A22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ECB8D9D-BBC9-4376-834D-D2903A9AC0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>https://docs.microsoft.com/en-gb/learn/modules/provision-virtual-machines-azure/</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Scheduled</t>
+  </si>
+  <si>
+    <t>Session 4</t>
+  </si>
+  <si>
+    <t>Session 5</t>
   </si>
 </sst>
 </file>
@@ -123,7 +129,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -151,6 +157,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFB9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -182,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -196,9 +208,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -230,6 +239,15 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -520,7 +538,7 @@
   <dimension ref="B2:H29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.6" x14ac:dyDescent="0.3"/>
@@ -537,44 +555,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="13"/>
+      <c r="E3" s="12"/>
       <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="4" t="s">
@@ -585,240 +603,248 @@
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="7"/>
-      <c r="C6" s="5" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="13" t="s">
-        <v>7</v>
+      <c r="D6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>20</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="7"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="6"/>
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="13" t="s">
+      <c r="D7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="7"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="15"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="14"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>2</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3"/>
-      <c r="E9" s="13"/>
+      <c r="E9" s="12"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>20</v>
+      <c r="E10" s="18" t="s">
+        <v>19</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="7"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="16" t="s">
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="15" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-      <c r="C12" s="5" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="13" t="s">
+      <c r="D12" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="6"/>
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>7</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="15"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="14"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="12"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
+      <c r="B16" s="6"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="12"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="12"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="13"/>
+      <c r="E18" s="12"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="13"/>
+      <c r="E19" s="12"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
+      <c r="B20" s="6"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="13"/>
+      <c r="E20" s="12"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
+      <c r="B21" s="6"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="13"/>
+      <c r="E21" s="12"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="12"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="12"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="13"/>
+      <c r="E24" s="12"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="12"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="12"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
+      <c r="B27" s="6"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="12"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="13"/>
+      <c r="E28" s="12"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="12"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
     </row>

</xml_diff>